<commit_message>
small cleanup input format
</commit_message>
<xml_diff>
--- a/F1.xlsx
+++ b/F1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daan\PycharmProjects\F1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\f1_fantasy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1DB5480-2C52-4C52-88C6-17D9A525E752}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFB1545C-913B-4B37-A118-6DFD74F96886}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="1215" windowWidth="17235" windowHeight="14385" activeTab="1" xr2:uid="{9ED39436-AE6A-4FFC-A319-A677D24087A8}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9ED39436-AE6A-4FFC-A319-A677D24087A8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="37">
   <si>
     <t>Name</t>
   </si>
@@ -113,9 +113,6 @@
     <t>Shadowcopy</t>
   </si>
   <si>
-    <t>F. lap</t>
-  </si>
-  <si>
     <t>Constructor</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
   </si>
   <si>
     <t>RAC</t>
-  </si>
-  <si>
-    <t>Constructor price</t>
   </si>
 </sst>
 </file>
@@ -501,10 +495,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C4AAD414-A20E-4A0D-83DE-455C4E3BF37A}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="C37" sqref="C37"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="C37" sqref="A33:C37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -738,17 +732,6 @@
         <v>20</v>
       </c>
       <c r="C32">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>26</v>
-      </c>
-      <c r="B34" t="s">
-        <v>22</v>
-      </c>
-      <c r="C34">
         <v>1</v>
       </c>
     </row>
@@ -772,10 +755,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B6F11DD-EE45-486C-9FE8-5728F5DFFE78}">
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -786,7 +769,7 @@
     <col min="5" max="5" width="17.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -797,13 +780,10 @@
         <v>24</v>
       </c>
       <c r="D1" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -815,14 +795,10 @@
         <v>1</v>
       </c>
       <c r="D2" t="s">
-        <v>28</v>
-      </c>
-      <c r="E2">
-        <f>(MATCH(D2,Constructors!A2:A11,0))</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
@@ -834,10 +810,10 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
@@ -849,10 +825,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
@@ -864,10 +840,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -879,10 +855,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -894,10 +870,10 @@
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
@@ -909,10 +885,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
@@ -924,10 +900,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
@@ -939,10 +915,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -954,10 +930,10 @@
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
@@ -969,10 +945,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
@@ -984,10 +960,10 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
@@ -999,10 +975,10 @@
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>17</v>
       </c>
@@ -1014,10 +990,10 @@
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>18</v>
       </c>
@@ -1029,7 +1005,7 @@
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -1044,7 +1020,7 @@
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
@@ -1059,7 +1035,7 @@
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
@@ -1074,7 +1050,7 @@
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
@@ -1089,7 +1065,7 @@
         <v>0</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
@@ -1104,7 +1080,7 @@
         <v>0</v>
       </c>
       <c r="D21" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -1133,7 +1109,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B2">
         <v>9.5</v>
@@ -1141,7 +1117,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B3">
         <v>25</v>
@@ -1149,7 +1125,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B4">
         <v>7.4</v>
@@ -1157,7 +1133,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B5">
         <v>32</v>
@@ -1165,7 +1141,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>9.6999999999999993</v>
@@ -1173,7 +1149,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B7">
         <v>6.2</v>
@@ -1181,7 +1157,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B8">
         <v>12.5</v>
@@ -1189,7 +1165,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B9">
         <v>9.5</v>
@@ -1197,7 +1173,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B10">
         <v>6</v>
@@ -1205,7 +1181,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>29</v>

</xml_diff>